<commit_message>
6th and 7th test cases
</commit_message>
<xml_diff>
--- a/data/test_cases.xlsx
+++ b/data/test_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/53a66839347cb57d/Desktop/pythonProject/PostgresDataTestingFramework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{DE5DDFA7-7570-4AE3-93A4-C6026CC78FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12336168-05F1-4B78-869E-6E78AF9E5803}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{DE5DDFA7-7570-4AE3-93A4-C6026CC78FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9060BB1F-909C-4F08-ADAC-5312C5BE8314}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B779F38F-EEA6-4973-A3E5-21E46716A4E6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B779F38F-EEA6-4973-A3E5-21E46716A4E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Total Order Placed By Category</t>
   </si>
   <si>
-    <t>% of Orders Dropped by Month</t>
-  </si>
-  <si>
     <t>Total Orders Placed By Year</t>
   </si>
   <si>
@@ -67,51 +64,18 @@
     <t>SELECT COUNT(*) FROM superstore_data;</t>
   </si>
   <si>
-    <t>CHECK_SCHEMA:superstore_data</t>
-  </si>
-  <si>
     <t>SELECT region, COUNT(*) FROM superstore_data GROUP BY region;</t>
   </si>
   <si>
     <t>SELECT category, COUNT(*) FROM superstore_data GROUP BY category;</t>
   </si>
   <si>
-    <t>SELECT EXTRACT(YEAR FROM order_date), COUNT(*) FROM superstore_data GROUP BY 1;</t>
-  </si>
-  <si>
-    <t>SELECT EXTRACT(YEAR FROM order_date), SUM(profit) FROM superstore_data GROUP BY 1;</t>
-  </si>
-  <si>
     <t>csv_count</t>
   </si>
   <si>
-    <t>CUSTOM:monthly_drop</t>
-  </si>
-  <si>
-    <t>compare_counts</t>
-  </si>
-  <si>
-    <t>{"order_id":"object","order_date":"object","region":"object","category":"object","profit":"float64"}</t>
-  </si>
-  <si>
-    <t>["order_id"," customer_id"," product_id"]</t>
-  </si>
-  <si>
     <t>CHECK_NOT_NULL:superstore_data</t>
   </si>
   <si>
-    <t>csv_groupby_year:order_id</t>
-  </si>
-  <si>
-    <t>csv_groupby_year:profit</t>
-  </si>
-  <si>
-    <t>csv_groupby:region</t>
-  </si>
-  <si>
-    <t>csv_groupby:category</t>
-  </si>
-  <si>
     <t>csv_groupby:Region</t>
   </si>
   <si>
@@ -134,6 +98,9 @@
   </si>
   <si>
     <t>{"order_id":"text","order_date":"text","region":"text","category":"text","profit":"double_precision"}</t>
+  </si>
+  <si>
+    <t>["Order ID","Customer ID","Product ID"]</t>
   </si>
 </sst>
 </file>
@@ -508,7 +475,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,10 +507,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -554,10 +521,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -568,10 +535,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -579,13 +546,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -593,13 +560,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -610,10 +577,24 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -650,108 +631,68 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD7"/>
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>